<commit_message>
changes are made in Excel too
</commit_message>
<xml_diff>
--- a/TimePass.xlsx
+++ b/TimePass.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -342,12 +342,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -358,7 +369,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -370,7 +381,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>